<commit_message>
Test missed off test plan for when both checkboxes are unchecked. Now added.
</commit_message>
<xml_diff>
--- a/_Project Documentation/Test plan/Test plan - Tyne & Wear Hospital Finder.xlsx
+++ b/_Project Documentation/Test plan/Test plan - Tyne & Wear Hospital Finder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="21075" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="21075" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Functional tests" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
   <si>
     <t>Test No.</t>
   </si>
@@ -38,9 +38,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>NR</t>
-  </si>
-  <si>
     <t>Functional tests</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Recheck the Hospitals checkboxes, uncheck the Departure Points checkbox, and click the Show Markers button. The map displays the Hospitals markers only, with a blue icon.</t>
   </si>
   <si>
-    <t>Using the default values in both checkboxes, click the Show Markers button. The interactive map displays the Departure Points markers with a red icon, and the Hospital markers with a blue icon.</t>
-  </si>
-  <si>
     <t>All the Departure Points and Hospitals are marked on map but with icons the same colour of blue i.e. there is no visual distinction between Departure Points markers and Hospital markers.</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>The active Routes tab displays the following: A heading appropriate to the Departure Area, Help text on finding routes, Departure Point, Destination Hospital, Travel Mode dropdown lists,  an unchecked Multiple Routes checkbox, a Find Route button, and a Clear Map button.</t>
   </si>
   <si>
-    <t>Click the Markers tab to make it active. The tab displays the following: A heading appropriate to the Departure Area, Help text on showing markers, checked checkbox for both Departure Points and Hospitals, a Show Markers button, and a Clear Map button.</t>
-  </si>
-  <si>
     <t>Click the Clear Map button. The map is cleared of all rendered routes and re-centered on the selected Departure Area. There should be no changes to the Tab panel.</t>
   </si>
   <si>
@@ -201,6 +192,18 @@
   </si>
   <si>
     <t>Yes. CSS styling class was applied in error to an #id in the HTML instead of to a class.</t>
+  </si>
+  <si>
+    <t>Using the default checked values in both checkboxes, click the Show Markers button. The interactive map displays the Departure Points markers with a red icon, and the Hospital markers with a blue icon.</t>
+  </si>
+  <si>
+    <t>Click the Markers tab to make it active. The tab displays the following: A heading appropriate to the Departure Area, Help text on showing markers, checked checkboxes for both Departure Points and Hospitals, a Show Markers button, and a Clear Map button.</t>
+  </si>
+  <si>
+    <t>Uncheck both checkboxes and click on Show Markers button. An alert displays warning that at least one checkbox must be checked.</t>
+  </si>
+  <si>
+    <t>Nothing happens. No markers are shown and no alert message appears.</t>
   </si>
 </sst>
 </file>
@@ -806,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -830,7 +833,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -842,7 +845,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -854,7 +857,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -866,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
@@ -883,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>2</v>
@@ -896,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
@@ -909,7 +912,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
@@ -922,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
@@ -935,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
@@ -948,13 +951,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -963,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>2</v>
@@ -976,7 +979,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
@@ -989,7 +992,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>2</v>
@@ -1002,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>2</v>
@@ -1015,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>1</v>
@@ -1032,7 +1035,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>2</v>
@@ -1045,7 +1048,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2</v>
@@ -1058,7 +1061,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>2</v>
@@ -1071,13 +1074,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5"/>
     </row>
@@ -1086,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>2</v>
@@ -1099,7 +1102,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>2</v>
@@ -1112,7 +1115,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>2</v>
@@ -1125,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>1</v>
@@ -1142,7 +1145,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>2</v>
@@ -1155,16 +1158,16 @@
         <v>19</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="45">
@@ -1172,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>2</v>
@@ -1185,7 +1188,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>2</v>
@@ -1198,13 +1201,30 @@
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" ht="45">
+      <c r="A32" s="7">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1222,7 +1242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1260,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1255,7 +1275,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -1271,7 +1291,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1280,7 +1300,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -1295,19 +1315,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>3</v>
@@ -1321,13 +1341,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>2</v>
@@ -1343,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
@@ -1365,13 +1385,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>2</v>
@@ -1387,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
@@ -1409,13 +1429,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>2</v>
@@ -1431,13 +1451,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>2</v>
@@ -1453,19 +1473,19 @@
         <v>0</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>3</v>
@@ -1479,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>2</v>
@@ -1501,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>2</v>
@@ -1523,7 +1543,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
@@ -1538,10 +1558,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30">
@@ -1549,19 +1569,19 @@
         <v>0</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>3</v>
@@ -1575,7 +1595,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2</v>
@@ -1597,7 +1617,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>2</v>
@@ -1619,7 +1639,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>

</xml_diff>